<commit_message>
all import in extra row remove
</commit_message>
<xml_diff>
--- a/new-invoice-frontend/main/src/assets/files/clientimport.xlsx
+++ b/new-invoice-frontend/main/src/assets/files/clientimport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\rovuk-invoice\new-invoice-frontend\main\src\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -759,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -796,19 +796,23 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="1"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -817,10 +821,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -829,10 +833,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -841,10 +845,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -853,7 +857,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>14</v>
@@ -865,10 +869,10 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -877,10 +881,10 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -889,7 +893,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>19</v>
@@ -901,10 +905,10 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -913,10 +917,10 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -925,10 +929,10 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -937,10 +941,10 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -949,10 +953,10 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -961,35 +965,31 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+        <v>24</v>
+      </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>19</v>
@@ -997,15 +997,15 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>27</v>
@@ -1013,15 +1013,15 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>9</v>
@@ -1029,7 +1029,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>9</v>
@@ -1037,7 +1037,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>9</v>
@@ -1045,31 +1045,31 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>9</v>
@@ -1077,23 +1077,23 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>27</v>
@@ -1101,7 +1101,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>27</v>
@@ -1109,31 +1109,31 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>27</v>
@@ -1141,23 +1141,23 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>27</v>
@@ -1165,7 +1165,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>27</v>
@@ -1173,39 +1173,39 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>27</v>
@@ -1213,15 +1213,15 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>17</v>
@@ -1229,7 +1229,7 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>17</v>
@@ -1237,31 +1237,31 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>22</v>
@@ -1269,81 +1269,73 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
-    <hyperlink ref="B5" r:id="rId2"/>
-    <hyperlink ref="B6" r:id="rId3"/>
-    <hyperlink ref="B7" r:id="rId4"/>
-    <hyperlink ref="B8" r:id="rId5"/>
-    <hyperlink ref="B10" r:id="rId6"/>
-    <hyperlink ref="B11" r:id="rId7"/>
-    <hyperlink ref="B12" r:id="rId8"/>
-    <hyperlink ref="B13" r:id="rId9"/>
-    <hyperlink ref="B14" r:id="rId10"/>
-    <hyperlink ref="B15" r:id="rId11"/>
-    <hyperlink ref="B16" r:id="rId12"/>
-    <hyperlink ref="B17" r:id="rId13"/>
-    <hyperlink ref="B18" r:id="rId14"/>
-    <hyperlink ref="B19" r:id="rId15"/>
-    <hyperlink ref="B20" r:id="rId16"/>
-    <hyperlink ref="B21" r:id="rId17"/>
-    <hyperlink ref="B22" r:id="rId18"/>
-    <hyperlink ref="B23" r:id="rId19"/>
-    <hyperlink ref="B24" r:id="rId20"/>
-    <hyperlink ref="B25" r:id="rId21"/>
-    <hyperlink ref="B26" r:id="rId22"/>
-    <hyperlink ref="B27" r:id="rId23"/>
-    <hyperlink ref="B28" r:id="rId24"/>
-    <hyperlink ref="B29" r:id="rId25"/>
-    <hyperlink ref="B30" r:id="rId26"/>
-    <hyperlink ref="B31" r:id="rId27"/>
-    <hyperlink ref="B32" r:id="rId28"/>
-    <hyperlink ref="B33" r:id="rId29"/>
-    <hyperlink ref="B34" r:id="rId30"/>
-    <hyperlink ref="B35" r:id="rId31"/>
-    <hyperlink ref="B36" r:id="rId32"/>
-    <hyperlink ref="B37" r:id="rId33"/>
-    <hyperlink ref="B38" r:id="rId34"/>
-    <hyperlink ref="B39" r:id="rId35"/>
-    <hyperlink ref="B40" r:id="rId36"/>
-    <hyperlink ref="B41" r:id="rId37"/>
-    <hyperlink ref="B42" r:id="rId38"/>
-    <hyperlink ref="B43" r:id="rId39"/>
-    <hyperlink ref="B44" r:id="rId40"/>
-    <hyperlink ref="B45" r:id="rId41"/>
-    <hyperlink ref="B46" r:id="rId42"/>
-    <hyperlink ref="B47" r:id="rId43"/>
-    <hyperlink ref="B49" r:id="rId44"/>
-    <hyperlink ref="B50" r:id="rId45"/>
-    <hyperlink ref="B51" r:id="rId46"/>
-    <hyperlink ref="B52" r:id="rId47"/>
-    <hyperlink ref="B53" r:id="rId48"/>
-    <hyperlink ref="B54" r:id="rId49"/>
-    <hyperlink ref="B55" r:id="rId50"/>
-    <hyperlink ref="B56" r:id="rId51"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B6" r:id="rId4"/>
+    <hyperlink ref="B7" r:id="rId5"/>
+    <hyperlink ref="B9" r:id="rId6"/>
+    <hyperlink ref="B10" r:id="rId7"/>
+    <hyperlink ref="B11" r:id="rId8"/>
+    <hyperlink ref="B12" r:id="rId9"/>
+    <hyperlink ref="B13" r:id="rId10"/>
+    <hyperlink ref="B14" r:id="rId11"/>
+    <hyperlink ref="B15" r:id="rId12"/>
+    <hyperlink ref="B16" r:id="rId13"/>
+    <hyperlink ref="B17" r:id="rId14"/>
+    <hyperlink ref="B18" r:id="rId15"/>
+    <hyperlink ref="B19" r:id="rId16"/>
+    <hyperlink ref="B20" r:id="rId17"/>
+    <hyperlink ref="B21" r:id="rId18"/>
+    <hyperlink ref="B22" r:id="rId19"/>
+    <hyperlink ref="B23" r:id="rId20"/>
+    <hyperlink ref="B24" r:id="rId21"/>
+    <hyperlink ref="B25" r:id="rId22"/>
+    <hyperlink ref="B26" r:id="rId23"/>
+    <hyperlink ref="B27" r:id="rId24"/>
+    <hyperlink ref="B28" r:id="rId25"/>
+    <hyperlink ref="B29" r:id="rId26"/>
+    <hyperlink ref="B30" r:id="rId27"/>
+    <hyperlink ref="B31" r:id="rId28"/>
+    <hyperlink ref="B32" r:id="rId29"/>
+    <hyperlink ref="B33" r:id="rId30"/>
+    <hyperlink ref="B34" r:id="rId31"/>
+    <hyperlink ref="B35" r:id="rId32"/>
+    <hyperlink ref="B36" r:id="rId33"/>
+    <hyperlink ref="B37" r:id="rId34"/>
+    <hyperlink ref="B38" r:id="rId35"/>
+    <hyperlink ref="B39" r:id="rId36"/>
+    <hyperlink ref="B40" r:id="rId37"/>
+    <hyperlink ref="B41" r:id="rId38"/>
+    <hyperlink ref="B42" r:id="rId39"/>
+    <hyperlink ref="B43" r:id="rId40"/>
+    <hyperlink ref="B44" r:id="rId41"/>
+    <hyperlink ref="B45" r:id="rId42"/>
+    <hyperlink ref="B46" r:id="rId43"/>
+    <hyperlink ref="B48" r:id="rId44"/>
+    <hyperlink ref="B49" r:id="rId45"/>
+    <hyperlink ref="B50" r:id="rId46"/>
+    <hyperlink ref="B51" r:id="rId47"/>
+    <hyperlink ref="B52" r:id="rId48"/>
+    <hyperlink ref="B53" r:id="rId49"/>
+    <hyperlink ref="B54" r:id="rId50"/>
+    <hyperlink ref="B55" r:id="rId51"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>